<commit_message>
whit grades and boxplots
</commit_message>
<xml_diff>
--- a/data/WQ_Variables.xlsx
+++ b/data/WQ_Variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z5282148\Desktop\whitsundays\r-rivers2reef\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brie.sherow\Desktop\R\r-rivers2reef\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF18CC63-97CA-4323-A854-3F8AB8FC1D3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6AB12A0-09C0-4DE2-98A1-9B71BEEF0252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29745" yWindow="735" windowWidth="18075" windowHeight="9495" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23970" yWindow="3420" windowWidth="16185" windowHeight="10455" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sites" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1538" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1538" uniqueCount="178">
   <si>
     <t>Partner</t>
   </si>
@@ -616,6 +616,9 @@
   </si>
   <si>
     <t>Dry 2, Wet 12</t>
+  </si>
+  <si>
+    <t>NTU</t>
   </si>
 </sst>
 </file>
@@ -1708,12 +1711,12 @@
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="29.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1733,12 +1736,12 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1758,7 +1761,7 @@
         <v>148.13999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1778,7 +1781,7 @@
         <v>148.01</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1798,7 +1801,7 @@
         <v>147.94</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1818,7 +1821,7 @@
         <v>147.91</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1838,7 +1841,7 @@
         <v>148.36000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1858,7 +1861,7 @@
         <v>148.72</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1878,7 +1881,7 @@
         <v>148.88999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1898,7 +1901,7 @@
         <v>149.04</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1918,7 +1921,7 @@
         <v>148.71</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1938,7 +1941,7 @@
         <v>148.86000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -1958,7 +1961,7 @@
         <v>149.34</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1978,7 +1981,7 @@
         <v>149.30000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -1998,7 +2001,7 @@
         <v>149.26</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -2018,7 +2021,7 @@
         <v>149.24</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -2038,7 +2041,7 @@
         <v>149.25</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -2058,7 +2061,7 @@
         <v>149.30000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -2078,7 +2081,7 @@
         <v>149.32</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -2098,7 +2101,7 @@
         <v>149.41999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -2112,7 +2115,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -2126,7 +2129,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>45</v>
       </c>
@@ -2140,7 +2143,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -2154,7 +2157,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -2168,7 +2171,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -2196,26 +2199,26 @@
       <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="21.90625" customWidth="1"/>
-    <col min="4" max="4" width="12.26953125" customWidth="1"/>
-    <col min="5" max="5" width="23.54296875" customWidth="1"/>
-    <col min="6" max="6" width="12.08984375" customWidth="1"/>
-    <col min="7" max="7" width="19.26953125" customWidth="1"/>
-    <col min="8" max="8" width="11.7265625" customWidth="1"/>
-    <col min="9" max="9" width="10.453125" customWidth="1"/>
-    <col min="10" max="10" width="10.1796875" customWidth="1"/>
-    <col min="11" max="11" width="12.453125" customWidth="1"/>
-    <col min="12" max="12" width="11.54296875" customWidth="1"/>
-    <col min="13" max="13" width="11.26953125" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="21.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" customWidth="1"/>
     <col min="14" max="15" width="12" customWidth="1"/>
-    <col min="16" max="16" width="8.90625" customWidth="1"/>
-    <col min="18" max="18" width="44.1796875" customWidth="1"/>
+    <col min="16" max="16" width="8.85546875" customWidth="1"/>
+    <col min="18" max="18" width="44.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>108</v>
       </c>
@@ -2271,7 +2274,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>109</v>
       </c>
@@ -2318,7 +2321,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2368,7 +2371,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2418,7 +2421,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -2468,7 +2471,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -2518,7 +2521,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -2568,7 +2571,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -2618,7 +2621,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -2668,7 +2671,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -2718,7 +2721,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>111</v>
       </c>
@@ -2753,7 +2756,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -2803,7 +2806,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -2850,7 +2853,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -2900,7 +2903,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -2947,7 +2950,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -2997,7 +3000,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -3047,7 +3050,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -3097,7 +3100,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -3144,7 +3147,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>44</v>
       </c>
@@ -3194,7 +3197,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -3244,7 +3247,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -3294,7 +3297,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>52</v>
       </c>
@@ -3362,34 +3365,34 @@
       <selection activeCell="C1" sqref="C1:J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.453125" customWidth="1"/>
-    <col min="4" max="4" width="9.1796875" customWidth="1"/>
-    <col min="7" max="7" width="9.90625" customWidth="1"/>
-    <col min="9" max="9" width="10.7265625" customWidth="1"/>
-    <col min="10" max="10" width="19.26953125" customWidth="1"/>
-    <col min="11" max="11" width="16.26953125" customWidth="1"/>
-    <col min="12" max="12" width="16.6328125" customWidth="1"/>
-    <col min="13" max="13" width="12.7265625" customWidth="1"/>
-    <col min="14" max="14" width="11.453125" customWidth="1"/>
-    <col min="15" max="15" width="11.1796875" customWidth="1"/>
-    <col min="16" max="16" width="13.453125" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" customWidth="1"/>
+    <col min="12" max="12" width="16.5703125" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" customWidth="1"/>
+    <col min="16" max="16" width="13.42578125" customWidth="1"/>
     <col min="17" max="17" width="12" customWidth="1"/>
-    <col min="18" max="18" width="14.26953125" customWidth="1"/>
-    <col min="19" max="19" width="16.6328125" customWidth="1"/>
-    <col min="20" max="20" width="14.7265625" customWidth="1"/>
-    <col min="21" max="21" width="13.7265625" customWidth="1"/>
-    <col min="22" max="22" width="13.453125" customWidth="1"/>
-    <col min="23" max="23" width="15.7265625" customWidth="1"/>
-    <col min="24" max="24" width="14.26953125" customWidth="1"/>
-    <col min="25" max="25" width="16.54296875" customWidth="1"/>
-    <col min="26" max="26" width="18.90625" customWidth="1"/>
+    <col min="18" max="18" width="14.28515625" customWidth="1"/>
+    <col min="19" max="19" width="16.5703125" customWidth="1"/>
+    <col min="20" max="20" width="14.7109375" customWidth="1"/>
+    <col min="21" max="21" width="13.7109375" customWidth="1"/>
+    <col min="22" max="22" width="13.42578125" customWidth="1"/>
+    <col min="23" max="23" width="15.7109375" customWidth="1"/>
+    <col min="24" max="24" width="14.28515625" customWidth="1"/>
+    <col min="25" max="25" width="16.5703125" customWidth="1"/>
+    <col min="26" max="26" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>134</v>
       </c>
@@ -3469,7 +3472,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -3544,7 +3547,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -3619,7 +3622,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -3694,7 +3697,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -3769,7 +3772,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -3844,7 +3847,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -3919,7 +3922,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -3994,7 +3997,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -4069,7 +4072,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -4114,7 +4117,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -4189,7 +4192,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -4258,7 +4261,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -4330,7 +4333,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -4399,7 +4402,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -4471,7 +4474,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -4543,7 +4546,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -4615,7 +4618,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -4684,7 +4687,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -4759,7 +4762,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -4834,7 +4837,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -4909,7 +4912,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -4999,12 +5002,12 @@
   <dimension ref="A1:F148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -5024,7 +5027,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -5044,7 +5047,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -5064,7 +5067,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -5084,7 +5087,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -5104,7 +5107,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -5124,7 +5127,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -5144,7 +5147,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -5164,7 +5167,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -5184,7 +5187,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -5204,7 +5207,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -5221,7 +5224,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -5238,7 +5241,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -5258,7 +5261,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -5275,7 +5278,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -5295,7 +5298,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -5315,7 +5318,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -5335,7 +5338,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -5352,7 +5355,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -5372,7 +5375,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -5392,7 +5395,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -5412,7 +5415,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -5432,7 +5435,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -5452,7 +5455,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -5472,7 +5475,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -5492,7 +5495,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -5512,7 +5515,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -5532,7 +5535,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>18</v>
       </c>
@@ -5552,7 +5555,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>20</v>
       </c>
@@ -5572,7 +5575,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>22</v>
       </c>
@@ -5592,7 +5595,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>25</v>
       </c>
@@ -5609,7 +5612,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>27</v>
       </c>
@@ -5629,7 +5632,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -5649,7 +5652,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>31</v>
       </c>
@@ -5669,7 +5672,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -5689,7 +5692,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -5709,7 +5712,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -5729,7 +5732,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -5749,7 +5752,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>41</v>
       </c>
@@ -5769,7 +5772,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>43</v>
       </c>
@@ -5789,7 +5792,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -5809,7 +5812,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>49</v>
       </c>
@@ -5829,7 +5832,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>51</v>
       </c>
@@ -5849,7 +5852,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -5869,7 +5872,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -5889,7 +5892,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>10</v>
       </c>
@@ -5909,7 +5912,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>12</v>
       </c>
@@ -5929,7 +5932,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>14</v>
       </c>
@@ -5949,7 +5952,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>18</v>
       </c>
@@ -5969,7 +5972,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>20</v>
       </c>
@@ -5989,7 +5992,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>22</v>
       </c>
@@ -6009,7 +6012,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>25</v>
       </c>
@@ -6026,7 +6029,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>27</v>
       </c>
@@ -6046,7 +6049,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>29</v>
       </c>
@@ -6066,7 +6069,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>31</v>
       </c>
@@ -6086,7 +6089,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>33</v>
       </c>
@@ -6106,7 +6109,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>35</v>
       </c>
@@ -6126,7 +6129,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>37</v>
       </c>
@@ -6146,7 +6149,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>39</v>
       </c>
@@ -6166,7 +6169,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>41</v>
       </c>
@@ -6186,7 +6189,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>43</v>
       </c>
@@ -6206,7 +6209,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>47</v>
       </c>
@@ -6226,7 +6229,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>49</v>
       </c>
@@ -6246,7 +6249,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>51</v>
       </c>
@@ -6266,7 +6269,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>6</v>
       </c>
@@ -6286,7 +6289,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>8</v>
       </c>
@@ -6306,7 +6309,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>10</v>
       </c>
@@ -6326,7 +6329,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>12</v>
       </c>
@@ -6346,7 +6349,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>14</v>
       </c>
@@ -6366,7 +6369,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>18</v>
       </c>
@@ -6386,7 +6389,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>20</v>
       </c>
@@ -6406,7 +6409,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>22</v>
       </c>
@@ -6426,7 +6429,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>25</v>
       </c>
@@ -6446,7 +6449,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>27</v>
       </c>
@@ -6466,7 +6469,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>29</v>
       </c>
@@ -6486,7 +6489,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>31</v>
       </c>
@@ -6506,7 +6509,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>33</v>
       </c>
@@ -6526,7 +6529,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>35</v>
       </c>
@@ -6546,7 +6549,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>37</v>
       </c>
@@ -6566,7 +6569,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>39</v>
       </c>
@@ -6586,7 +6589,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>41</v>
       </c>
@@ -6606,7 +6609,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>43</v>
       </c>
@@ -6626,7 +6629,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>47</v>
       </c>
@@ -6646,7 +6649,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>49</v>
       </c>
@@ -6666,7 +6669,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>51</v>
       </c>
@@ -6686,7 +6689,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>6</v>
       </c>
@@ -6706,7 +6709,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>8</v>
       </c>
@@ -6726,7 +6729,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>10</v>
       </c>
@@ -6746,7 +6749,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>12</v>
       </c>
@@ -6766,7 +6769,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>14</v>
       </c>
@@ -6786,7 +6789,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>18</v>
       </c>
@@ -6806,7 +6809,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>20</v>
       </c>
@@ -6826,7 +6829,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>22</v>
       </c>
@@ -6846,7 +6849,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>25</v>
       </c>
@@ -6863,7 +6866,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>27</v>
       </c>
@@ -6883,7 +6886,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>29</v>
       </c>
@@ -6903,7 +6906,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>31</v>
       </c>
@@ -6923,7 +6926,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>33</v>
       </c>
@@ -6943,7 +6946,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>35</v>
       </c>
@@ -6963,7 +6966,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>37</v>
       </c>
@@ -6983,7 +6986,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>39</v>
       </c>
@@ -7003,7 +7006,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>41</v>
       </c>
@@ -7023,7 +7026,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>43</v>
       </c>
@@ -7043,7 +7046,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>47</v>
       </c>
@@ -7063,7 +7066,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>49</v>
       </c>
@@ -7083,7 +7086,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>51</v>
       </c>
@@ -7103,7 +7106,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>6</v>
       </c>
@@ -7123,7 +7126,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>8</v>
       </c>
@@ -7143,7 +7146,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>10</v>
       </c>
@@ -7163,7 +7166,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>12</v>
       </c>
@@ -7183,7 +7186,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>14</v>
       </c>
@@ -7203,7 +7206,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>18</v>
       </c>
@@ -7223,7 +7226,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>20</v>
       </c>
@@ -7243,7 +7246,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>22</v>
       </c>
@@ -7263,7 +7266,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>25</v>
       </c>
@@ -7280,7 +7283,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>27</v>
       </c>
@@ -7300,7 +7303,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>29</v>
       </c>
@@ -7320,7 +7323,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>31</v>
       </c>
@@ -7340,7 +7343,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>33</v>
       </c>
@@ -7360,7 +7363,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>35</v>
       </c>
@@ -7380,7 +7383,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>37</v>
       </c>
@@ -7400,7 +7403,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>39</v>
       </c>
@@ -7420,7 +7423,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>41</v>
       </c>
@@ -7440,7 +7443,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>43</v>
       </c>
@@ -7460,7 +7463,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>47</v>
       </c>
@@ -7480,7 +7483,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>49</v>
       </c>
@@ -7500,7 +7503,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>51</v>
       </c>
@@ -7520,7 +7523,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>6</v>
       </c>
@@ -7528,7 +7531,7 @@
         <v>7</v>
       </c>
       <c r="C128" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="D128">
         <v>1</v>
@@ -7540,7 +7543,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>8</v>
       </c>
@@ -7548,7 +7551,7 @@
         <v>9</v>
       </c>
       <c r="C129" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="D129">
         <v>1</v>
@@ -7560,7 +7563,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>10</v>
       </c>
@@ -7568,7 +7571,7 @@
         <v>11</v>
       </c>
       <c r="C130" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="D130">
         <v>1</v>
@@ -7580,7 +7583,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>12</v>
       </c>
@@ -7588,7 +7591,7 @@
         <v>13</v>
       </c>
       <c r="C131" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="D131">
         <v>1</v>
@@ -7600,7 +7603,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>14</v>
       </c>
@@ -7608,7 +7611,7 @@
         <v>15</v>
       </c>
       <c r="C132" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="D132">
         <v>1</v>
@@ -7620,7 +7623,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>18</v>
       </c>
@@ -7628,7 +7631,7 @@
         <v>19</v>
       </c>
       <c r="C133" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="D133">
         <v>1.1000000000000001</v>
@@ -7640,7 +7643,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>20</v>
       </c>
@@ -7648,7 +7651,7 @@
         <v>21</v>
       </c>
       <c r="C134" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="D134">
         <v>1.1000000000000001</v>
@@ -7660,7 +7663,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>22</v>
       </c>
@@ -7668,7 +7671,7 @@
         <v>23</v>
       </c>
       <c r="C135" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="D135">
         <v>1.1000000000000001</v>
@@ -7680,7 +7683,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>25</v>
       </c>
@@ -7688,7 +7691,7 @@
         <v>26</v>
       </c>
       <c r="C136" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="D136" t="s">
         <v>159</v>
@@ -7697,7 +7700,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>27</v>
       </c>
@@ -7705,7 +7708,7 @@
         <v>28</v>
       </c>
       <c r="C137" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="D137">
         <v>1.1000000000000001</v>
@@ -7717,7 +7720,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>29</v>
       </c>
@@ -7725,7 +7728,7 @@
         <v>30</v>
       </c>
       <c r="C138" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="D138">
         <v>1</v>
@@ -7737,7 +7740,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>31</v>
       </c>
@@ -7745,7 +7748,7 @@
         <v>32</v>
       </c>
       <c r="C139" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="D139" t="s">
         <v>176</v>
@@ -7757,7 +7760,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>33</v>
       </c>
@@ -7765,7 +7768,7 @@
         <v>34</v>
       </c>
       <c r="C140" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="D140">
         <v>1</v>
@@ -7777,7 +7780,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>35</v>
       </c>
@@ -7785,7 +7788,7 @@
         <v>36</v>
       </c>
       <c r="C141" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="D141" t="s">
         <v>176</v>
@@ -7797,7 +7800,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>37</v>
       </c>
@@ -7805,7 +7808,7 @@
         <v>38</v>
       </c>
       <c r="C142" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="D142" t="s">
         <v>176</v>
@@ -7817,7 +7820,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>39</v>
       </c>
@@ -7825,7 +7828,7 @@
         <v>40</v>
       </c>
       <c r="C143" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="D143" t="s">
         <v>176</v>
@@ -7837,7 +7840,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>41</v>
       </c>
@@ -7845,7 +7848,7 @@
         <v>42</v>
       </c>
       <c r="C144" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="D144">
         <v>1</v>
@@ -7857,7 +7860,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>43</v>
       </c>
@@ -7865,7 +7868,7 @@
         <v>44</v>
       </c>
       <c r="C145" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="D145">
         <v>1</v>
@@ -7877,7 +7880,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>47</v>
       </c>
@@ -7885,7 +7888,7 @@
         <v>133</v>
       </c>
       <c r="C146" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="D146">
         <v>1</v>
@@ -7897,7 +7900,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>49</v>
       </c>
@@ -7905,7 +7908,7 @@
         <v>50</v>
       </c>
       <c r="C147" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="D147">
         <v>1</v>
@@ -7917,7 +7920,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>51</v>
       </c>
@@ -7925,7 +7928,7 @@
         <v>52</v>
       </c>
       <c r="C148" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="D148">
         <v>1</v>
@@ -7953,13 +7956,13 @@
       <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="12" max="12" width="10.26953125" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7997,7 +8000,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -8035,7 +8038,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -8073,7 +8076,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>167</v>
       </c>
@@ -8127,9 +8130,9 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -8137,7 +8140,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -8145,7 +8148,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -8153,7 +8156,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>

</xml_diff>